<commit_message>
Demais comandos linux, diretório e permissões.
</commit_message>
<xml_diff>
--- a/Documentos/Resumos/ListaDeComandosLinux.xlsx
+++ b/Documentos/Resumos/ListaDeComandosLinux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Arquivos\Estudo\TI\Linux\Documentos\Resumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{14AB1213-C3BA-49C9-A72F-356A1B966797}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4BBEAC81-336C-4AFD-8DA0-1720C19BC17E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="6045" xr2:uid="{93312C4E-1DA1-4B77-B43F-7A257DDAEB4F}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="GrupoDeComanodos" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Grupos">GrupoDeComanodos!$A$1:$A$8</definedName>
+    <definedName name="Grupos">GrupoDeComanodos!$A$1:$A$10</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
   <si>
     <t>Comando</t>
   </si>
@@ -184,6 +184,70 @@
   </si>
   <si>
     <t>du</t>
+  </si>
+  <si>
+    <t>apt</t>
+  </si>
+  <si>
+    <t>Instalação</t>
+  </si>
+  <si>
+    <t>sudo</t>
+  </si>
+  <si>
+    <t>apt-get</t>
+  </si>
+  <si>
+    <t>ls -l</t>
+  </si>
+  <si>
+    <t>chmod [opções] modo arquivo</t>
+  </si>
+  <si>
+    <t>addgroup</t>
+  </si>
+  <si>
+    <t>Grupos de Usuários</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Utilize o comando id sempre que quiser obter informações sobre um usuário
+do sistema. Ele irá retornar UID, GID e os grupos aos quais o usuário pertence.</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> delUser [usuario] [grupo]</t>
+  </si>
+  <si>
+    <t>adduser [usuario] [grupo]</t>
+  </si>
+  <si>
+    <t>chown</t>
+  </si>
+  <si>
+    <t>chgrp [grupo] [arquivo]</t>
+  </si>
+  <si>
+    <t>aptitude</t>
+  </si>
+  <si>
+    <t>add-apt-repository</t>
+  </si>
+  <si>
+    <t>sudo apt-get install build-essential</t>
+  </si>
+  <si>
+    <t>sudo apt-get install apache2</t>
+  </si>
+  <si>
+    <t>apt-cache</t>
+  </si>
+  <si>
+    <t>Sempre que quiser obter informações sobre um pacote</t>
   </si>
 </sst>
 </file>
@@ -539,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC5D29A-F8DA-4F1C-BC74-190A9666113C}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,6 +898,112 @@
         <v>21</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B98" xr:uid="{2A326FC0-BB6A-4F5B-8F57-D2AD0BCCFCDD}">
@@ -846,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B6F9F4-F19B-4BF3-B8B0-49AC68064685}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,6 +1067,16 @@
         <v>37</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>